<commit_message>
sample data and custume package for NineChronicles
</commit_message>
<xml_diff>
--- a/tables/xlsx/Character/Character.xlsx
+++ b/tables/xlsx/Character/Character.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maste\Projects\Planetarium\NineChronicles\tables\xlsx\Character\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9500EE2C-46A6-4487-A855-CD73B155BCE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C5433AB-E25B-4D8A-9879-18AF9C4E0973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5805" yWindow="3735" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{0A762577-43D9-46EB-BC68-64F699260E26}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="21525" windowHeight="11820" xr2:uid="{0A762577-43D9-46EB-BC68-64F699260E26}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="3" r:id="rId1"/>
@@ -727,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5970BEC-BA53-493B-96D8-33B18D9A690E}">
   <dimension ref="A1:R60"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4122,8 +4122,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08E5372C-F45A-44DD-9D42-5FF902DBF4B0}">
   <dimension ref="A1:C401"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C1"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>